<commit_message>
seperate view and logic
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="100" windowWidth="19200" windowHeight="11640" tabRatio="735"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="19200" windowHeight="11640" tabRatio="735" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="171">
   <si>
     <t>view.grid.size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,22 +154,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>edge.w</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>edge.color</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>半径</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>body.radius</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>颜色</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -226,14 +214,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>body.color</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>body.playerColor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>duration</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -307,14 +287,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>边数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>side</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>radius</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -327,14 +299,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>勾边颜色</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>edge.color</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x555555</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -467,14 +431,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>宽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -491,22 +447,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>颜色</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>射击位置偏移</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>w</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bullet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -515,10 +459,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>color</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>shootOffset</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -578,50 +518,6 @@
     <t>0x999999</t>
   </si>
   <si>
-    <t>xOffsetRatio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yOffsetRatio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xDisplayRatio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yDisplayRatio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>alpha</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>圆角半径</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>透明度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x偏移比例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y偏移比例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x显示缩放</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y显示缩放</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x86c680</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -654,14 +550,166 @@
   </si>
   <si>
     <t>每帧放大比例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.edge.w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.edge.color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示半径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.body.radius</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.body.color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.body.playerColor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>半径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>radius</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示边数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示半径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示颜色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示勾边宽度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示勾边颜色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.side</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.radius</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>radius</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示宽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.edge.color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.edge.w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示勾边宽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.edge.w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.颜色(己方)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.body.playerColor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>血条显示宽度比例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>血条显示高度比例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示圆角半径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示透明度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.alpha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>血条显示x偏移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>血条显示y偏移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.hpbar.scaleXRatio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.hpbar.scaleYRatio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.hpbar.xOffsetRatio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view.hpbar.yOffsetRatio</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,7 +744,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -706,6 +754,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,7 +805,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -770,9 +836,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1063,21 +1138,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="7.125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="2"/>
+    <col min="4" max="6" width="21.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="21.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1">
@@ -1180,19 +1255,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1">
@@ -1249,169 +1324,176 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" customWidth="1"/>
+    <col min="12" max="12" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="N1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="O1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="R1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="7" customFormat="1">
+      <c r="A2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="H2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="I2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" s="7" customFormat="1">
-      <c r="A2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="K2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="2" customFormat="1">
+      <c r="A3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" s="2" customFormat="1">
-      <c r="A3" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1">
         <v>900</v>
@@ -1426,37 +1508,40 @@
         <v>1</v>
       </c>
       <c r="K3" s="1">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1">
         <v>300</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>200</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>300</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>200</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>80</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>100</v>
       </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
       <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
         <v>30</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1466,149 +1551,182 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5" customWidth="1"/>
+    <col min="15" max="15" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:23">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="B1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="Q1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="R1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="T1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="U1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="V1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="7" customFormat="1">
+      <c r="A2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="L2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="7" customFormat="1">
-      <c r="A2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="M2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" s="2" customFormat="1">
+      <c r="V2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -1617,54 +1735,69 @@
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1">
         <v>2.5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="K3" s="1">
         <v>20</v>
       </c>
-      <c r="H3" s="1">
+      <c r="L3" s="1">
         <v>2</v>
       </c>
-      <c r="I3" s="1">
+      <c r="M3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1">
+      <c r="N3" s="1">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1">
         <v>3</v>
       </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
         <v>3</v>
       </c>
-      <c r="M3" s="1">
+      <c r="R3" s="1">
         <v>3</v>
       </c>
-      <c r="N3" s="1">
+      <c r="S3" s="1">
         <v>80</v>
       </c>
-      <c r="O3" s="1">
+      <c r="T3" s="1">
         <v>120</v>
       </c>
-      <c r="P3" s="1">
+      <c r="U3" s="1">
         <v>0.5</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="V3" s="1">
         <v>30</v>
       </c>
-      <c r="R3" s="1">
+      <c r="W3" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
@@ -1673,54 +1806,69 @@
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E4" s="1">
         <v>2.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="K4" s="1">
         <v>40</v>
       </c>
-      <c r="H4" s="1">
+      <c r="L4" s="1">
         <v>4</v>
       </c>
-      <c r="I4" s="1">
+      <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
+      <c r="N4" s="1">
+        <v>20</v>
+      </c>
+      <c r="O4" s="1">
         <v>3</v>
       </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
         <v>3</v>
       </c>
-      <c r="M4" s="1">
+      <c r="R4" s="1">
         <v>3</v>
       </c>
-      <c r="N4" s="1">
+      <c r="S4" s="1">
         <v>80</v>
       </c>
-      <c r="O4" s="1">
+      <c r="T4" s="1">
         <v>100</v>
       </c>
-      <c r="P4" s="1">
+      <c r="U4" s="1">
         <v>0.5</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="V4" s="1">
         <v>30</v>
       </c>
-      <c r="R4" s="1">
+      <c r="W4" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:23">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -1729,48 +1877,63 @@
         <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1">
         <v>2.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="K5" s="1">
         <v>80</v>
       </c>
-      <c r="H5" s="1">
+      <c r="L5" s="1">
         <v>8</v>
       </c>
-      <c r="I5" s="1">
+      <c r="M5" s="1">
         <v>1</v>
       </c>
-      <c r="J5" s="1">
+      <c r="N5" s="1">
+        <v>24</v>
+      </c>
+      <c r="O5" s="1">
         <v>3</v>
       </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
         <v>3</v>
       </c>
-      <c r="M5" s="1">
+      <c r="R5" s="1">
         <v>3</v>
       </c>
-      <c r="N5" s="1">
+      <c r="S5" s="1">
         <v>80</v>
       </c>
-      <c r="O5" s="1">
+      <c r="T5" s="1">
         <v>80</v>
       </c>
-      <c r="P5" s="1">
+      <c r="U5" s="1">
         <v>0.5</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="V5" s="1">
         <v>30</v>
       </c>
-      <c r="R5" s="1">
+      <c r="W5" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1786,364 +1949,443 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.375" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5" customWidth="1"/>
+    <col min="15" max="15" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:27">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="B1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="M1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="Q1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="R1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="T1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="U1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="V1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="7" customFormat="1">
+      <c r="A2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="L2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" s="7" customFormat="1">
-      <c r="A2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="N2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="P2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="V2" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" s="2" customFormat="1">
+      <c r="W2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1">
         <v>2.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1">
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="K3" s="1">
         <v>200</v>
       </c>
-      <c r="H3" s="1">
+      <c r="L3" s="1">
         <v>10</v>
       </c>
-      <c r="I3" s="1">
+      <c r="M3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="N3" s="1">
+        <v>24</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
         <v>400</v>
       </c>
-      <c r="L3" s="1">
+      <c r="Q3" s="1">
         <v>160</v>
       </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
         <v>80</v>
       </c>
-      <c r="O3" s="1">
+      <c r="T3" s="1">
         <v>120</v>
       </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
         <v>30</v>
       </c>
-      <c r="R3" s="1">
+      <c r="W3" s="1">
         <v>10</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="X3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1">
         <v>2.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D4" s="1">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="K4" s="1">
         <v>300</v>
       </c>
-      <c r="H4" s="1">
+      <c r="L4" s="1">
         <v>10</v>
       </c>
-      <c r="I4" s="1">
+      <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="N4" s="1">
+        <v>26</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
         <v>400</v>
       </c>
-      <c r="L4" s="1">
+      <c r="Q4" s="1">
         <v>160</v>
       </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
         <v>80</v>
       </c>
-      <c r="O4" s="1">
+      <c r="T4" s="1">
         <v>120</v>
       </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
         <v>30</v>
       </c>
-      <c r="R4" s="1">
+      <c r="W4" s="1">
         <v>10</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="X4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B5" s="1">
         <v>2.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1">
-        <v>400</v>
+        <v>0.6</v>
       </c>
       <c r="H5" s="1">
-        <v>10</v>
+        <v>0.6</v>
       </c>
       <c r="I5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="K5" s="1">
         <v>400</v>
       </c>
       <c r="L5" s="1">
+        <v>10</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>26</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q5" s="1">
         <v>160</v>
       </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
         <v>80</v>
       </c>
-      <c r="O5" s="1">
+      <c r="T5" s="1">
         <v>120</v>
       </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
         <v>30</v>
       </c>
-      <c r="R5" s="1">
+      <c r="W5" s="1">
         <v>10</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>98</v>
+      <c r="X5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2159,121 +2401,138 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.25" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1">
+    <row r="1" spans="1:17" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="7" customFormat="1">
+      <c r="A2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="N2" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="O2" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="7" customFormat="1">
-      <c r="A2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1">
         <v>15</v>
@@ -2281,46 +2540,52 @@
       <c r="C3" s="1">
         <v>35</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
+      <c r="D3" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>45</v>
+      </c>
+      <c r="L3" s="1">
         <v>10</v>
       </c>
-      <c r="J3" s="1">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
         <v>3</v>
       </c>
-      <c r="L3" s="1">
+      <c r="N3" s="1">
         <v>15</v>
       </c>
-      <c r="M3" s="1">
+      <c r="O3" s="1">
         <v>10000</v>
       </c>
-      <c r="N3" s="1">
+      <c r="P3" s="1">
         <v>16</v>
       </c>
-      <c r="O3" s="1">
+      <c r="Q3" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -2328,46 +2593,52 @@
       <c r="C4" s="1">
         <v>40</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="1">
         <v>-8</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>50</v>
+      </c>
+      <c r="L4" s="1">
         <v>10</v>
       </c>
-      <c r="J4" s="1">
-        <v>10</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
         <v>3</v>
       </c>
-      <c r="L4" s="1">
+      <c r="N4" s="1">
         <v>15</v>
       </c>
-      <c r="M4" s="1">
+      <c r="O4" s="1">
         <v>8000</v>
       </c>
-      <c r="N4" s="1">
+      <c r="P4" s="1">
         <v>16</v>
       </c>
-      <c r="O4" s="1">
+      <c r="Q4" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1">
         <v>12</v>
@@ -2375,46 +2646,52 @@
       <c r="C5" s="1">
         <v>40</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="1">
         <v>8</v>
       </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>50</v>
+      </c>
+      <c r="L5" s="1">
         <v>10</v>
       </c>
-      <c r="J5" s="1">
-        <v>10</v>
-      </c>
-      <c r="K5" s="1">
+      <c r="M5" s="1">
         <v>6</v>
       </c>
-      <c r="L5" s="1">
+      <c r="N5" s="1">
         <v>15</v>
       </c>
-      <c r="M5" s="1">
+      <c r="O5" s="1">
         <v>8000</v>
       </c>
-      <c r="N5" s="1">
+      <c r="P5" s="1">
         <v>16</v>
       </c>
-      <c r="O5" s="1">
+      <c r="Q5" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B6" s="1">
         <v>16</v>
@@ -2422,46 +2699,52 @@
       <c r="C6" s="1">
         <v>38</v>
       </c>
-      <c r="D6" s="1">
-        <v>0</v>
+      <c r="D6" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>48</v>
+      </c>
+      <c r="L6" s="1">
         <v>10</v>
       </c>
-      <c r="J6" s="1">
-        <v>10</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="M6" s="1">
         <v>3</v>
       </c>
-      <c r="L6" s="1">
+      <c r="N6" s="1">
         <v>15</v>
       </c>
-      <c r="M6" s="1">
+      <c r="O6" s="1">
         <v>10000</v>
       </c>
-      <c r="N6" s="1">
+      <c r="P6" s="1">
         <v>16</v>
       </c>
-      <c r="O6" s="1">
+      <c r="Q6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B7" s="1">
         <v>16</v>
@@ -2469,46 +2752,52 @@
       <c r="C7" s="1">
         <v>38</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
+      <c r="D7" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="1">
         <v>90</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="K7" s="1">
+        <v>48</v>
+      </c>
+      <c r="L7" s="1">
         <v>10</v>
       </c>
-      <c r="J7" s="1">
-        <v>10</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="M7" s="1">
         <v>6</v>
       </c>
-      <c r="L7" s="1">
+      <c r="N7" s="1">
         <v>15</v>
       </c>
-      <c r="M7" s="1">
+      <c r="O7" s="1">
         <v>10000</v>
       </c>
-      <c r="N7" s="1">
+      <c r="P7" s="1">
         <v>16</v>
       </c>
-      <c r="O7" s="1">
+      <c r="Q7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1">
         <v>16</v>
@@ -2516,46 +2805,52 @@
       <c r="C8" s="1">
         <v>38</v>
       </c>
-      <c r="D8" s="1">
-        <v>0</v>
+      <c r="D8" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" s="1">
         <v>180</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="K8" s="1">
+        <v>48</v>
+      </c>
+      <c r="L8" s="1">
         <v>10</v>
       </c>
-      <c r="J8" s="1">
-        <v>10</v>
-      </c>
-      <c r="K8" s="1">
+      <c r="M8" s="1">
         <v>3</v>
       </c>
-      <c r="L8" s="1">
+      <c r="N8" s="1">
         <v>15</v>
       </c>
-      <c r="M8" s="1">
+      <c r="O8" s="1">
         <v>10000</v>
       </c>
-      <c r="N8" s="1">
+      <c r="P8" s="1">
         <v>16</v>
       </c>
-      <c r="O8" s="1">
+      <c r="Q8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B9" s="1">
         <v>16</v>
@@ -2563,40 +2858,46 @@
       <c r="C9" s="1">
         <v>38</v>
       </c>
-      <c r="D9" s="1">
-        <v>0</v>
+      <c r="D9" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J9" s="1">
         <v>270</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="K9" s="1">
+        <v>48</v>
+      </c>
+      <c r="L9" s="1">
         <v>10</v>
       </c>
-      <c r="J9" s="1">
-        <v>10</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="M9" s="1">
         <v>6</v>
       </c>
-      <c r="L9" s="1">
+      <c r="N9" s="1">
         <v>15</v>
       </c>
-      <c r="M9" s="1">
+      <c r="O9" s="1">
         <v>10000</v>
       </c>
-      <c r="N9" s="1">
+      <c r="P9" s="1">
         <v>16</v>
       </c>
-      <c r="O9" s="1">
+      <c r="Q9" s="1">
         <v>5</v>
       </c>
     </row>
@@ -2613,110 +2914,84 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" customWidth="1"/>
-    <col min="5" max="5" width="5.5" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1">
+    <row r="1" spans="1:8" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="D1" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="9" customFormat="1">
+      <c r="A2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="G2" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="9" customFormat="1">
-      <c r="A2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1">
         <v>100</v>
@@ -2728,22 +3003,10 @@
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="H3" s="1">
         <v>0.75</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -2759,19 +3022,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2780,38 +3043,38 @@
         <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1">
       <c r="A2" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1">
         <v>0.4</v>

</xml_diff>

<commit_message>
change directory to use node.js
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="19200" windowHeight="11640" tabRatio="735" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="23940" windowHeight="15100" tabRatio="735" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="176">
   <si>
     <t>view.grid.size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -210,10 +210,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>自旋初值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>duration</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -254,10 +250,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>velocity.rotation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x555555</t>
   </si>
   <si>
@@ -710,14 +702,34 @@
   </si>
   <si>
     <t>velocity.ivDec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>velocity.rv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自旋速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自旋速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>velocity.rv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>velocity.rv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,6 +760,24 @@
       <color theme="4"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -808,8 +838,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -854,8 +890,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1146,21 +1184,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="7.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="21.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="2"/>
+    <col min="4" max="6" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1">
@@ -1263,19 +1301,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1">
@@ -1332,31 +1370,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView showGridLines="0" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1371,7 +1409,7 @@
         <v>31</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>34</v>
@@ -1392,7 +1430,7 @@
         <v>39</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>41</v>
@@ -1401,7 +1439,7 @@
         <v>40</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="O1" s="11" t="s">
         <v>42</v>
@@ -1416,98 +1454,98 @@
         <v>45</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>46</v>
+        <v>172</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="7" customFormat="1">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="S2" s="6" t="s">
-        <v>57</v>
+        <v>171</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="1">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="G3" s="1">
         <v>900</v>
@@ -1558,7 +1596,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1568,35 +1606,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView showGridLines="0" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.625" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="15" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1604,31 +1642,31 @@
         <v>29</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>145</v>
-      </c>
       <c r="G1" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>37</v>
@@ -1649,7 +1687,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R1" s="11" t="s">
         <v>42</v>
@@ -1664,92 +1702,92 @@
         <v>45</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="X1" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="7" customFormat="1">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="O2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="U2" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="V2" s="6" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -1758,13 +1796,13 @@
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E3" s="1">
         <v>2.5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G3" s="1">
         <v>0.6</v>
@@ -1823,7 +1861,7 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
@@ -1832,13 +1870,13 @@
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E4" s="1">
         <v>2.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G4" s="1">
         <v>0.6</v>
@@ -1897,7 +1935,7 @@
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -1906,13 +1944,13 @@
         <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1">
         <v>2.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G5" s="1">
         <v>0.6</v>
@@ -1981,38 +2019,38 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.625" customWidth="1"/>
-    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.375" customWidth="1"/>
+    <col min="9" max="10" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="15" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="21" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -2020,31 +2058,31 @@
         <v>29</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>160</v>
-      </c>
       <c r="H1" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>37</v>
@@ -2065,7 +2103,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R1" s="11" t="s">
         <v>42</v>
@@ -2080,131 +2118,131 @@
         <v>45</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>46</v>
+        <v>172</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="X1" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="7" customFormat="1">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>159</v>
-      </c>
       <c r="G2" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="U2" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="V2" s="6" t="s">
-        <v>57</v>
+        <v>175</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Y2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1">
         <v>2.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1">
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="G3" s="1">
         <v>0.6</v>
@@ -2261,7 +2299,7 @@
         <v>10</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
@@ -2269,22 +2307,22 @@
     </row>
     <row r="4" spans="1:28">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="1">
         <v>2.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="1">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G4" s="1">
         <v>0.6</v>
@@ -2341,32 +2379,32 @@
         <v>10</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
     <row r="5" spans="1:28">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1">
         <v>2.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" s="1">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="G5" s="1">
         <v>0.6</v>
@@ -2423,16 +2461,16 @@
         <v>10</v>
       </c>
       <c r="Y5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2448,27 +2486,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.25" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="4" customFormat="1">
@@ -2476,110 +2514,110 @@
         <v>29</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>106</v>
-      </c>
       <c r="L1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M1" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="P1" s="11" t="s">
-        <v>118</v>
-      </c>
       <c r="Q1" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="7" customFormat="1">
       <c r="A2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>103</v>
-      </c>
       <c r="I2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="N2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="P2" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1">
         <v>15</v>
@@ -2588,13 +2626,13 @@
         <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -2603,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -2632,7 +2670,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -2641,13 +2679,13 @@
         <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G4" s="1">
         <v>-8</v>
@@ -2656,7 +2694,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -2685,7 +2723,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1">
         <v>12</v>
@@ -2694,13 +2732,13 @@
         <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G5" s="1">
         <v>8</v>
@@ -2709,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
@@ -2738,7 +2776,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B6" s="1">
         <v>16</v>
@@ -2747,13 +2785,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -2762,7 +2800,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
@@ -2791,7 +2829,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1">
         <v>16</v>
@@ -2800,13 +2838,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -2815,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J7" s="1">
         <v>90</v>
@@ -2844,7 +2882,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" s="1">
         <v>16</v>
@@ -2853,13 +2891,13 @@
         <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -2868,7 +2906,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J8" s="1">
         <v>180</v>
@@ -2897,7 +2935,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" s="1">
         <v>16</v>
@@ -2906,13 +2944,13 @@
         <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -2921,7 +2959,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J9" s="1">
         <v>270</v>
@@ -2961,21 +2999,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
@@ -2983,62 +3021,62 @@
         <v>29</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="9" customFormat="1">
       <c r="A2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1">
         <v>100</v>
@@ -3050,7 +3088,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H3" s="1">
         <v>0.75</v>
@@ -3069,19 +3107,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3090,38 +3128,38 @@
         <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1">
       <c r="A2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1">
         <v>0.4</v>

</xml_diff>

<commit_message>
name bar display config
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="23940" windowHeight="15100" tabRatio="735" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="23940" windowHeight="15100" tabRatio="735" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="190">
   <si>
     <t>view.grid.size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -722,6 +722,61 @@
   </si>
   <si>
     <t>velocity.rv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>namebar.font</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18px Arail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19px Arail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字显示字体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字显示填充色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字显示沟边色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字显示沟边宽度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x101010</t>
+  </si>
+  <si>
+    <t>0xf0f0f0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>namebar.fill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>namebar.stroke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>namebar.strokeThickness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字显示高度偏移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>namebar.yOffset</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -782,7 +837,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -813,6 +868,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -838,7 +899,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -848,8 +909,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -889,10 +968,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2020,10 +2108,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="V1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2048,12 +2136,16 @@
     <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="21" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:33">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -2126,20 +2218,35 @@
       <c r="X1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="7" customFormat="1">
+    <row r="2" spans="1:33" s="7" customFormat="1">
       <c r="A2" s="6" t="s">
         <v>57</v>
       </c>
@@ -2213,19 +2320,34 @@
         <v>91</v>
       </c>
       <c r="Y2" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1">
+    <row r="3" spans="1:33" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -2299,13 +2421,28 @@
         <v>10</v>
       </c>
       <c r="Y3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>15</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:33">
       <c r="A4" s="1" t="s">
         <v>73</v>
       </c>
@@ -2379,15 +2516,30 @@
         <v>10</v>
       </c>
       <c r="Y4" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>18</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:33">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -2461,15 +2613,30 @@
         <v>10</v>
       </c>
       <c r="Y5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>18</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AG5" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3110,7 +3277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add lock-step: move & rotation operation
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22950" windowHeight="9945" tabRatio="735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22950" windowHeight="9945" tabRatio="735" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
@@ -1166,7 +1166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="X1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -2180,7 +2180,7 @@
         <v>120</v>
       </c>
       <c r="W3" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X3" s="4">
         <v>30</v>
@@ -2278,7 +2278,7 @@
         <v>120</v>
       </c>
       <c r="W4" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X4" s="4">
         <v>30</v>
@@ -2378,7 +2378,7 @@
         <v>120</v>
       </c>
       <c r="W5" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X5" s="4">
         <v>30</v>

</xml_diff>

<commit_message>
add sync force & rotation interval
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22950" windowHeight="9945" tabRatio="735" activeTab="4"/>
+    <workbookView xWindow="3160" yWindow="520" windowWidth="23440" windowHeight="13220" tabRatio="735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,17 @@
     <sheet name="configDieAnimation" sheetId="8" r:id="rId8"/>
     <sheet name="configPropAdd" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="191">
   <si>
     <t>地图宽</t>
   </si>
@@ -586,14 +591,30 @@
   </si>
   <si>
     <t>unitCollideCheckFrame</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>syncRotationFrame</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>syncForceFrame</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步移动间隔(帧)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步旋转间隔(帧)</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,10 +781,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -1051,21 +1072,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="7.125" style="7" customWidth="1"/>
+    <col min="1" max="2" width="7.1640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="11" style="7" customWidth="1"/>
-    <col min="4" max="6" width="21.375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="23.875" style="7" customWidth="1"/>
-    <col min="8" max="9" width="21.375" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="7"/>
+    <col min="4" max="6" width="21.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" style="7" customWidth="1"/>
+    <col min="8" max="9" width="21.33203125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1">
@@ -1159,99 +1180,129 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="21.375" customWidth="1"/>
-    <col min="3" max="3" width="23.625" customWidth="1"/>
-    <col min="4" max="4" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1">
+    <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="16" customFormat="1">
+    <row r="2" spans="1:6" s="16" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="7" customFormat="1">
+    <row r="3" spans="1:6" s="7" customFormat="1">
       <c r="A3" s="4">
         <v>30</v>
       </c>
       <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
         <v>128</v>
       </c>
-      <c r="C3" s="4">
+      <c r="E3" s="4">
         <v>15</v>
       </c>
-      <c r="D3" s="4">
+      <c r="F3" s="4">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="4" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="6" width="24.375" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.125" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" customWidth="1"/>
     <col min="9" max="9" width="7.5" customWidth="1"/>
     <col min="10" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="17.125" customWidth="1"/>
-    <col min="13" max="14" width="16.125" customWidth="1"/>
-    <col min="15" max="16" width="17.125" customWidth="1"/>
-    <col min="17" max="17" width="16.125" customWidth="1"/>
-    <col min="18" max="18" width="17.125" customWidth="1"/>
-    <col min="19" max="19" width="11.625" customWidth="1"/>
-    <col min="20" max="20" width="22.125" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" customWidth="1"/>
+    <col min="13" max="14" width="16.1640625" customWidth="1"/>
+    <col min="15" max="16" width="17.1640625" customWidth="1"/>
+    <col min="17" max="17" width="16.1640625" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" customWidth="1"/>
+    <col min="20" max="20" width="22.1640625" customWidth="1"/>
     <col min="21" max="21" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1454,38 +1505,43 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.625" customWidth="1"/>
-    <col min="2" max="2" width="11.125" customWidth="1"/>
-    <col min="3" max="3" width="13.125" customWidth="1"/>
-    <col min="4" max="4" width="11.125" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="17.625" customWidth="1"/>
-    <col min="7" max="8" width="24.375" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="8" width="24.33203125" customWidth="1"/>
     <col min="9" max="10" width="25.5" customWidth="1"/>
-    <col min="11" max="11" width="7.125" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" customWidth="1"/>
     <col min="12" max="12" width="7.5" customWidth="1"/>
     <col min="13" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="15" width="17.125" customWidth="1"/>
-    <col min="16" max="17" width="16.125" customWidth="1"/>
-    <col min="18" max="19" width="17.125" customWidth="1"/>
-    <col min="20" max="20" width="16.125" customWidth="1"/>
-    <col min="21" max="21" width="16.375" customWidth="1"/>
-    <col min="22" max="22" width="11.625" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" customWidth="1"/>
+    <col min="16" max="17" width="16.1640625" customWidth="1"/>
+    <col min="18" max="19" width="17.1640625" customWidth="1"/>
+    <col min="20" max="20" width="16.1640625" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
     <col min="23" max="23" width="19" customWidth="1"/>
-    <col min="24" max="24" width="18.125" customWidth="1"/>
+    <col min="24" max="24" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1861,47 +1917,52 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="P1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.625" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="4" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="7" width="24.375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="25.5" customWidth="1"/>
-    <col min="9" max="10" width="26.625" customWidth="1"/>
-    <col min="11" max="11" width="10.375" customWidth="1"/>
+    <col min="9" max="10" width="26.6640625" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
     <col min="14" max="14" width="8.5" customWidth="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="17.125" customWidth="1"/>
-    <col min="17" max="18" width="16.125" customWidth="1"/>
-    <col min="19" max="20" width="17.125" customWidth="1"/>
-    <col min="21" max="21" width="16.125" customWidth="1"/>
-    <col min="22" max="22" width="17.125" customWidth="1"/>
-    <col min="23" max="23" width="11.625" customWidth="1"/>
-    <col min="24" max="24" width="22.125" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" customWidth="1"/>
+    <col min="17" max="18" width="16.1640625" customWidth="1"/>
+    <col min="19" max="20" width="17.1640625" customWidth="1"/>
+    <col min="21" max="21" width="16.1640625" customWidth="1"/>
+    <col min="22" max="22" width="17.1640625" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="24" max="24" width="22.1640625" customWidth="1"/>
     <col min="25" max="25" width="21" customWidth="1"/>
-    <col min="26" max="26" width="12.625" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" customWidth="1"/>
     <col min="27" max="28" width="14.5" customWidth="1"/>
-    <col min="29" max="29" width="22.625" customWidth="1"/>
-    <col min="30" max="30" width="16.375" customWidth="1"/>
-    <col min="31" max="31" width="11.125" customWidth="1"/>
-    <col min="32" max="32" width="11.625" customWidth="1"/>
-    <col min="33" max="34" width="11.125" customWidth="1"/>
+    <col min="29" max="29" width="22.6640625" customWidth="1"/>
+    <col min="30" max="30" width="16.33203125" customWidth="1"/>
+    <col min="31" max="31" width="11.1640625" customWidth="1"/>
+    <col min="32" max="32" width="11.6640625" customWidth="1"/>
+    <col min="33" max="34" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -2418,31 +2479,36 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.625" customWidth="1"/>
-    <col min="4" max="4" width="17.625" customWidth="1"/>
-    <col min="5" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
-    <col min="7" max="7" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="12.625" customWidth="1"/>
-    <col min="13" max="13" width="17.125" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="16" max="16" width="15.125" customWidth="1"/>
-    <col min="17" max="17" width="17.125" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1">
@@ -2926,25 +2992,30 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="13.125" customWidth="1"/>
-    <col min="7" max="8" width="12.125" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="8" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1">
@@ -3029,23 +3100,28 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3103,27 +3179,32 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.875" customWidth="1"/>
-    <col min="2" max="3" width="10.25" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="3" width="10.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="10.125" customWidth="1"/>
-    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.25">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="1" t="s">
         <v>163</v>
       </c>
@@ -3143,7 +3224,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="2" t="s">
         <v>169</v>
       </c>
@@ -3327,5 +3408,10 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add exp & level
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="520" windowWidth="23440" windowHeight="13220" tabRatio="735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="735" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="configHpbar" sheetId="7" r:id="rId7"/>
     <sheet name="configDieAnimation" sheetId="8" r:id="rId8"/>
     <sheet name="configPropAdd" sheetId="9" r:id="rId9"/>
+    <sheet name="configLevelUp" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="199">
   <si>
     <t>地图宽</t>
   </si>
@@ -579,46 +580,86 @@
   </si>
   <si>
     <t>durationFrame</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>degree</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>碰撞检测保护时长(帧)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>unitCollideCheckFrame</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>syncRotationFrame</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>syncForceFrame</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>同步移动间隔(帧)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>同步旋转间隔(帧)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>击杀经验</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>killExp</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>等级</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>经验</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能点</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillPoint</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -655,6 +696,22 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -722,19 +779,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -746,7 +809,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -755,19 +818,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -779,8 +842,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1177,9 +1245,385 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>70</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>130</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>170</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>210</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>250</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>300</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>350</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>400</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>450</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>500</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>570</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>640</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>710</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>780</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>850</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>930</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>1010</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>1090</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>1170</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>1250</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>1350</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>1450</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>1550</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>1650</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>1800</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1192,7 +1636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1267,7 +1711,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1502,7 +1946,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
   <extLst>
@@ -1515,10 +1959,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1534,17 +1978,18 @@
     <col min="11" max="11" width="7.1640625" customWidth="1"/>
     <col min="12" max="12" width="7.5" customWidth="1"/>
     <col min="13" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" customWidth="1"/>
-    <col min="16" max="17" width="16.1640625" customWidth="1"/>
-    <col min="18" max="19" width="17.1640625" customWidth="1"/>
-    <col min="20" max="20" width="16.1640625" customWidth="1"/>
-    <col min="21" max="21" width="16.33203125" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" customWidth="1"/>
-    <col min="23" max="23" width="19" customWidth="1"/>
-    <col min="24" max="24" width="18.1640625" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" customWidth="1"/>
+    <col min="17" max="18" width="16.1640625" customWidth="1"/>
+    <col min="19" max="20" width="17.1640625" customWidth="1"/>
+    <col min="21" max="21" width="16.1640625" customWidth="1"/>
+    <col min="22" max="22" width="16.33203125" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="24" max="24" width="19" customWidth="1"/>
+    <col min="25" max="25" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -1587,38 +2032,41 @@
       <c r="N1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="P1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="11" customFormat="1">
+    <row r="2" spans="1:25" s="11" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>48</v>
       </c>
@@ -1662,37 +2110,40 @@
         <v>57</v>
       </c>
       <c r="O2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="P2" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="S2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="T2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="X2" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="Y2" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="7" customFormat="1">
+    <row r="3" spans="1:25" s="7" customFormat="1">
       <c r="A3" s="4" t="s">
         <v>87</v>
       </c>
@@ -1736,37 +2187,40 @@
         <v>20</v>
       </c>
       <c r="O3" s="4">
+        <v>10</v>
+      </c>
+      <c r="P3" s="4">
         <v>3</v>
-      </c>
-      <c r="P3" s="4">
-        <v>0</v>
       </c>
       <c r="Q3" s="4">
         <v>0</v>
       </c>
       <c r="R3" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S3" s="4">
         <v>3</v>
       </c>
       <c r="T3" s="4">
+        <v>3</v>
+      </c>
+      <c r="U3" s="4">
         <v>80</v>
       </c>
-      <c r="U3" s="4">
+      <c r="V3" s="4">
         <v>120</v>
       </c>
-      <c r="V3" s="4">
+      <c r="W3" s="4">
         <v>0.5</v>
       </c>
-      <c r="W3" s="4">
+      <c r="X3" s="4">
         <v>30</v>
       </c>
-      <c r="X3" s="4">
+      <c r="Y3" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4" s="4" t="s">
         <v>89</v>
       </c>
@@ -1810,37 +2264,40 @@
         <v>20</v>
       </c>
       <c r="O4" s="4">
+        <v>20</v>
+      </c>
+      <c r="P4" s="4">
         <v>3</v>
-      </c>
-      <c r="P4" s="4">
-        <v>0</v>
       </c>
       <c r="Q4" s="4">
         <v>0</v>
       </c>
       <c r="R4" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S4" s="4">
         <v>3</v>
       </c>
       <c r="T4" s="4">
+        <v>3</v>
+      </c>
+      <c r="U4" s="4">
         <v>80</v>
       </c>
-      <c r="U4" s="4">
+      <c r="V4" s="4">
         <v>100</v>
       </c>
-      <c r="V4" s="4">
+      <c r="W4" s="4">
         <v>0.5</v>
       </c>
-      <c r="W4" s="4">
+      <c r="X4" s="4">
         <v>30</v>
       </c>
-      <c r="X4" s="4">
+      <c r="Y4" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5" s="4" t="s">
         <v>91</v>
       </c>
@@ -1884,38 +2341,41 @@
         <v>24</v>
       </c>
       <c r="O5" s="4">
+        <v>40</v>
+      </c>
+      <c r="P5" s="4">
         <v>3</v>
-      </c>
-      <c r="P5" s="4">
-        <v>0</v>
       </c>
       <c r="Q5" s="4">
         <v>0</v>
       </c>
       <c r="R5" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S5" s="4">
         <v>3</v>
       </c>
       <c r="T5" s="4">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="U5" s="4">
         <v>80</v>
       </c>
       <c r="V5" s="4">
+        <v>80</v>
+      </c>
+      <c r="W5" s="4">
         <v>0.5</v>
       </c>
-      <c r="W5" s="4">
+      <c r="X5" s="4">
         <v>30</v>
       </c>
-      <c r="X5" s="4">
+      <c r="Y5" s="4">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1929,7 +2389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="P1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
@@ -2476,7 +2936,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
   <extLst>
@@ -2989,7 +3449,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
@@ -3097,7 +3557,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
@@ -3177,7 +3637,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3192,7 +3652,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3405,7 +3865,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>

</xml_diff>

<commit_message>
mv hpbar to ui
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15615" tabRatio="735" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15615" tabRatio="735" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
@@ -13,10 +13,9 @@
     <sheet name="configObstacles" sheetId="4" r:id="rId4"/>
     <sheet name="configTanks" sheetId="5" r:id="rId5"/>
     <sheet name="configWeapons" sheetId="6" r:id="rId6"/>
-    <sheet name="configHpbar" sheetId="7" r:id="rId7"/>
-    <sheet name="configDieAnimation" sheetId="8" r:id="rId8"/>
-    <sheet name="configPropAdd" sheetId="9" r:id="rId9"/>
-    <sheet name="configLevelUp" sheetId="10" r:id="rId10"/>
+    <sheet name="configDieAnimation" sheetId="8" r:id="rId7"/>
+    <sheet name="configPropAdd" sheetId="9" r:id="rId8"/>
+    <sheet name="configLevelUp" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="190">
   <si>
     <t>地图宽</t>
   </si>
@@ -258,18 +257,6 @@
     <t>显示勾边颜色</t>
   </si>
   <si>
-    <t>血条显示宽度比例</t>
-  </si>
-  <si>
-    <t>血条显示高度比例</t>
-  </si>
-  <si>
-    <t>血条显示x偏移</t>
-  </si>
-  <si>
-    <t>血条显示y偏移</t>
-  </si>
-  <si>
     <t>view.side</t>
   </si>
   <si>
@@ -279,18 +266,6 @@
     <t>view.color</t>
   </si>
   <si>
-    <t>view.hpbar.scaleXRatio</t>
-  </si>
-  <si>
-    <t>view.hpbar.scaleYRatio</t>
-  </si>
-  <si>
-    <t>view.hpbar.xOffsetRatio</t>
-  </si>
-  <si>
-    <t>view.hpbar.yOffsetRatio</t>
-  </si>
-  <si>
     <t>triangle</t>
   </si>
   <si>
@@ -481,18 +456,6 @@
   </si>
   <si>
     <t>0x999999</t>
-  </si>
-  <si>
-    <t>显示圆角半径</t>
-  </si>
-  <si>
-    <t>显示透明度</t>
-  </si>
-  <si>
-    <t>view.alpha</t>
-  </si>
-  <si>
-    <t>0x86c680</t>
   </si>
   <si>
     <t>动画开始透明度</t>
@@ -1268,382 +1231,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="14.25">
-      <c r="A1" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.25">
-      <c r="A2" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>50</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>70</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>130</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>170</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>210</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>250</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>300</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>350</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>400</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>450</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>500</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>570</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>640</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>710</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>780</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>850</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>930</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>1010</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>1090</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>1170</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>1250</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>1350</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29">
-        <v>1450</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30">
-        <v>1550</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31">
-        <v>1650</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32">
-        <v>1800</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
@@ -1667,16 +1254,16 @@
         <v>21</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>23</v>
@@ -1687,16 +1274,16 @@
         <v>24</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>26</v>
@@ -1737,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
@@ -1798,7 +1385,7 @@
         <v>37</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>38</v>
@@ -1851,7 +1438,7 @@
         <v>53</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>54</v>
@@ -1860,13 +1447,13 @@
         <v>55</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="M2" s="13" t="s">
         <v>58</v>
@@ -1981,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -1995,24 +1582,22 @@
     <col min="4" max="4" width="11.125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="17.625" customWidth="1"/>
-    <col min="7" max="8" width="24.375" customWidth="1"/>
-    <col min="9" max="10" width="25.5" customWidth="1"/>
-    <col min="11" max="11" width="7.125" customWidth="1"/>
-    <col min="12" max="12" width="7.5" customWidth="1"/>
-    <col min="13" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="15" width="10.375" customWidth="1"/>
-    <col min="16" max="16" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.125" customWidth="1"/>
-    <col min="18" max="19" width="16.125" customWidth="1"/>
-    <col min="20" max="21" width="17.125" customWidth="1"/>
-    <col min="22" max="22" width="16.125" customWidth="1"/>
-    <col min="23" max="23" width="16.375" customWidth="1"/>
-    <col min="24" max="24" width="11.625" customWidth="1"/>
-    <col min="25" max="25" width="19" customWidth="1"/>
-    <col min="26" max="26" width="18.125" customWidth="1"/>
+    <col min="7" max="7" width="7.125" customWidth="1"/>
+    <col min="8" max="8" width="7.5" customWidth="1"/>
+    <col min="9" max="10" width="8.5" customWidth="1"/>
+    <col min="11" max="11" width="10.375" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.125" customWidth="1"/>
+    <col min="14" max="15" width="16.125" customWidth="1"/>
+    <col min="16" max="17" width="17.125" customWidth="1"/>
+    <col min="18" max="18" width="16.125" customWidth="1"/>
+    <col min="19" max="19" width="16.375" customWidth="1"/>
+    <col min="20" max="20" width="11.625" customWidth="1"/>
+    <col min="21" max="21" width="19" customWidth="1"/>
+    <col min="22" max="22" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:22">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -2031,79 +1616,67 @@
       <c r="F1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>79</v>
+      <c r="G1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>200</v>
+        <v>188</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="U1" s="12" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="V1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z1" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="11" customFormat="1">
+    <row r="2" spans="1:22" s="11" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>49</v>
@@ -2112,69 +1685,57 @@
         <v>50</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>54</v>
+        <v>180</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>55</v>
+        <v>189</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>192</v>
+        <v>60</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>201</v>
+        <v>61</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="S2" s="13" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="T2" s="13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="U2" s="13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z2" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="7" customFormat="1">
+    <row r="3" spans="1:22" s="7" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
@@ -2183,7 +1744,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E3" s="4">
         <v>2.5</v>
@@ -2192,69 +1753,57 @@
         <v>69</v>
       </c>
       <c r="G3" s="4">
-        <v>0.6</v>
+        <v>100</v>
       </c>
       <c r="H3" s="4">
-        <v>0.6</v>
+        <v>10</v>
       </c>
       <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4">
+        <v>10</v>
+      </c>
+      <c r="L3" s="4">
+        <v>300</v>
+      </c>
+      <c r="M3" s="4">
+        <v>3</v>
+      </c>
+      <c r="N3" s="4">
         <v>0</v>
       </c>
-      <c r="J3" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="K3" s="4">
-        <v>100</v>
-      </c>
-      <c r="L3" s="4">
-        <v>10</v>
-      </c>
-      <c r="M3" s="4">
-        <v>1</v>
-      </c>
-      <c r="N3" s="4">
-        <v>20</v>
-      </c>
       <c r="O3" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P3" s="4">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="Q3" s="4">
         <v>3</v>
       </c>
       <c r="R3" s="4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="S3" s="4">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="T3" s="4">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="U3" s="4">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="V3" s="4">
-        <v>80</v>
-      </c>
-      <c r="W3" s="4">
-        <v>120</v>
-      </c>
-      <c r="X3" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="Y3" s="4">
-        <v>30</v>
-      </c>
-      <c r="Z3" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:22">
       <c r="A4" s="4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
@@ -2263,7 +1812,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E4" s="4">
         <v>2.5</v>
@@ -2272,69 +1821,57 @@
         <v>69</v>
       </c>
       <c r="G4" s="4">
-        <v>0.6</v>
+        <v>400</v>
       </c>
       <c r="H4" s="4">
-        <v>0.6</v>
+        <v>20</v>
       </c>
       <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>20</v>
+      </c>
+      <c r="K4" s="4">
+        <v>20</v>
+      </c>
+      <c r="L4" s="4">
+        <v>600</v>
+      </c>
+      <c r="M4" s="4">
+        <v>3</v>
+      </c>
+      <c r="N4" s="4">
         <v>0</v>
       </c>
-      <c r="J4" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="K4" s="4">
-        <v>400</v>
-      </c>
-      <c r="L4" s="4">
-        <v>20</v>
-      </c>
-      <c r="M4" s="4">
-        <v>1</v>
-      </c>
-      <c r="N4" s="4">
-        <v>20</v>
-      </c>
       <c r="O4" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P4" s="4">
-        <v>600</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="4">
         <v>3</v>
       </c>
       <c r="R4" s="4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="S4" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T4" s="4">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="U4" s="4">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="V4" s="4">
-        <v>80</v>
-      </c>
-      <c r="W4" s="4">
-        <v>100</v>
-      </c>
-      <c r="X4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="Y4" s="4">
-        <v>30</v>
-      </c>
-      <c r="Z4" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:22">
       <c r="A5" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4">
         <v>5</v>
@@ -2343,7 +1880,7 @@
         <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E5" s="4">
         <v>2.5</v>
@@ -2352,63 +1889,51 @@
         <v>69</v>
       </c>
       <c r="G5" s="4">
-        <v>0.6</v>
+        <v>1000</v>
       </c>
       <c r="H5" s="4">
-        <v>0.6</v>
+        <v>180</v>
       </c>
       <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>24</v>
+      </c>
+      <c r="K5" s="4">
+        <v>40</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2000</v>
+      </c>
+      <c r="M5" s="4">
+        <v>3</v>
+      </c>
+      <c r="N5" s="4">
         <v>0</v>
       </c>
-      <c r="J5" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="K5" s="4">
-        <v>1000</v>
-      </c>
-      <c r="L5" s="4">
-        <v>180</v>
-      </c>
-      <c r="M5" s="4">
-        <v>1</v>
-      </c>
-      <c r="N5" s="4">
-        <v>24</v>
-      </c>
       <c r="O5" s="4">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="P5" s="4">
-        <v>2000</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="4">
         <v>3</v>
       </c>
       <c r="R5" s="4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="S5" s="4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T5" s="4">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="U5" s="4">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="V5" s="4">
-        <v>80</v>
-      </c>
-      <c r="W5" s="4">
-        <v>80</v>
-      </c>
-      <c r="X5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="Y5" s="4">
-        <v>30</v>
-      </c>
-      <c r="Z5" s="4">
         <v>10</v>
       </c>
     </row>
@@ -2425,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="J1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView showGridLines="0" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -2438,38 +1963,36 @@
     <col min="3" max="3" width="17.625" customWidth="1"/>
     <col min="4" max="4" width="18.875" customWidth="1"/>
     <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="7" width="24.375" customWidth="1"/>
-    <col min="8" max="8" width="25.5" customWidth="1"/>
-    <col min="9" max="10" width="26.625" customWidth="1"/>
-    <col min="11" max="11" width="10.375" customWidth="1"/>
-    <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.125" customWidth="1"/>
-    <col min="18" max="19" width="16.125" customWidth="1"/>
-    <col min="20" max="21" width="17.125" customWidth="1"/>
-    <col min="22" max="22" width="16.125" customWidth="1"/>
-    <col min="23" max="23" width="17.125" customWidth="1"/>
-    <col min="24" max="24" width="11.625" customWidth="1"/>
-    <col min="25" max="25" width="22.125" customWidth="1"/>
-    <col min="26" max="26" width="21" customWidth="1"/>
-    <col min="27" max="27" width="12.625" customWidth="1"/>
-    <col min="28" max="29" width="14.5" customWidth="1"/>
-    <col min="30" max="30" width="22.625" customWidth="1"/>
-    <col min="31" max="31" width="16.375" customWidth="1"/>
-    <col min="32" max="32" width="11.125" customWidth="1"/>
-    <col min="33" max="33" width="11.625" customWidth="1"/>
-    <col min="34" max="35" width="11.125" customWidth="1"/>
+    <col min="6" max="6" width="24.375" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="8.5" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.125" customWidth="1"/>
+    <col min="14" max="15" width="16.125" customWidth="1"/>
+    <col min="16" max="17" width="17.125" customWidth="1"/>
+    <col min="18" max="18" width="16.125" customWidth="1"/>
+    <col min="19" max="19" width="17.125" customWidth="1"/>
+    <col min="20" max="20" width="11.625" customWidth="1"/>
+    <col min="21" max="21" width="22.125" customWidth="1"/>
+    <col min="22" max="22" width="21" customWidth="1"/>
+    <col min="23" max="23" width="12.625" customWidth="1"/>
+    <col min="24" max="25" width="14.5" customWidth="1"/>
+    <col min="26" max="26" width="22.625" customWidth="1"/>
+    <col min="27" max="27" width="16.375" customWidth="1"/>
+    <col min="28" max="28" width="11.125" customWidth="1"/>
+    <col min="29" max="29" width="11.625" customWidth="1"/>
+    <col min="30" max="31" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:31">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>29</v>
@@ -2478,100 +2001,88 @@
         <v>30</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA1" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB1" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD1" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="AE1" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="AF1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI1" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" s="11" customFormat="1">
+      <c r="AC1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="11" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>48</v>
       </c>
@@ -2591,96 +2102,84 @@
         <v>53</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>55</v>
+        <v>189</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD2" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="P2" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z2" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AE2" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="AB2" s="13" t="s">
+    </row>
+    <row r="3" spans="1:31" s="7" customFormat="1">
+      <c r="A3" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF2" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="AG2" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH2" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI2" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" s="7" customFormat="1">
-      <c r="A3" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="B3" s="4">
         <v>2.5</v>
@@ -2698,90 +2197,78 @@
         <v>71</v>
       </c>
       <c r="G3" s="4">
-        <v>0.6</v>
+        <v>1800</v>
       </c>
       <c r="H3" s="4">
-        <v>0.6</v>
+        <v>450</v>
       </c>
       <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L3" s="4">
+        <v>99999</v>
+      </c>
+      <c r="M3" s="4">
         <v>0</v>
       </c>
-      <c r="J3" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="K3" s="4">
-        <v>1800</v>
-      </c>
-      <c r="L3" s="4">
-        <v>450</v>
-      </c>
-      <c r="M3" s="4">
-        <v>1</v>
-      </c>
       <c r="N3" s="4">
-        <v>24</v>
+        <v>400</v>
       </c>
       <c r="O3" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>200</v>
       </c>
       <c r="P3" s="4">
-        <v>99999</v>
+        <v>160</v>
       </c>
       <c r="Q3" s="4">
         <v>0</v>
       </c>
       <c r="R3" s="4">
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="S3" s="4">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="T3" s="4">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="U3" s="4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="V3" s="4">
-        <v>80</v>
-      </c>
-      <c r="W3" s="4">
-        <v>120</v>
-      </c>
-      <c r="X3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="4">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="Z3" s="4">
-        <v>10</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>114</v>
+        <v>2</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>15</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD3" s="4">
-        <v>2</v>
-      </c>
-      <c r="AE3" s="4">
-        <v>15</v>
-      </c>
-      <c r="AF3" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG3" s="4"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="4"/>
-    </row>
-    <row r="4" spans="1:35">
+        <v>105</v>
+      </c>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B4" s="4">
         <v>2.5</v>
@@ -2799,92 +2286,80 @@
         <v>71</v>
       </c>
       <c r="G4" s="4">
-        <v>0.6</v>
+        <v>2000</v>
       </c>
       <c r="H4" s="4">
-        <v>0.6</v>
+        <v>500</v>
       </c>
       <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>26</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L4" s="4">
+        <v>99999</v>
+      </c>
+      <c r="M4" s="4">
         <v>0</v>
       </c>
-      <c r="J4" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="K4" s="4">
-        <v>2000</v>
-      </c>
-      <c r="L4" s="4">
-        <v>500</v>
-      </c>
-      <c r="M4" s="4">
-        <v>1</v>
-      </c>
       <c r="N4" s="4">
-        <v>26</v>
+        <v>400</v>
       </c>
       <c r="O4" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>200</v>
       </c>
       <c r="P4" s="4">
-        <v>99999</v>
+        <v>160</v>
       </c>
       <c r="Q4" s="4">
         <v>0</v>
       </c>
       <c r="R4" s="4">
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="S4" s="4">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="T4" s="4">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="U4" s="4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="V4" s="4">
-        <v>80</v>
-      </c>
-      <c r="W4" s="4">
-        <v>120</v>
-      </c>
-      <c r="X4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="4">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="Z4" s="4">
-        <v>10</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>118</v>
+        <v>2</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>18</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD4" s="4">
-        <v>2</v>
-      </c>
-      <c r="AE4" s="4">
-        <v>18</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-    </row>
-    <row r="5" spans="1:35">
+        <v>112</v>
+      </c>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" s="4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B5" s="4">
         <v>2.5</v>
@@ -2902,91 +2377,79 @@
         <v>71</v>
       </c>
       <c r="G5" s="4">
-        <v>0.6</v>
+        <v>2200</v>
       </c>
       <c r="H5" s="4">
-        <v>0.6</v>
+        <v>550</v>
       </c>
       <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>26</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L5" s="4">
+        <v>99999</v>
+      </c>
+      <c r="M5" s="4">
         <v>0</v>
       </c>
-      <c r="J5" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="K5" s="4">
-        <v>2200</v>
-      </c>
-      <c r="L5" s="4">
-        <v>550</v>
-      </c>
-      <c r="M5" s="4">
-        <v>1</v>
-      </c>
       <c r="N5" s="4">
-        <v>26</v>
+        <v>400</v>
       </c>
       <c r="O5" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>200</v>
       </c>
       <c r="P5" s="4">
-        <v>99999</v>
+        <v>160</v>
       </c>
       <c r="Q5" s="4">
         <v>0</v>
       </c>
       <c r="R5" s="4">
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="S5" s="4">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="T5" s="4">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="U5" s="4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="V5" s="4">
-        <v>80</v>
-      </c>
-      <c r="W5" s="4">
-        <v>120</v>
-      </c>
-      <c r="X5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="4">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="Z5" s="4">
-        <v>10</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>118</v>
+        <v>2</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>18</v>
       </c>
       <c r="AB5" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD5" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AE5" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="AD5" s="4">
-        <v>2</v>
-      </c>
-      <c r="AE5" s="4">
-        <v>18</v>
-      </c>
-      <c r="AF5" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="AH5" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AI5" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3030,52 +2493,52 @@
         <v>27</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="N1" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>131</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="11" customFormat="1">
@@ -3083,10 +2546,10 @@
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>50</v>
@@ -3095,45 +2558,45 @@
         <v>49</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B3" s="4">
         <v>15</v>
@@ -3148,7 +2611,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -3186,7 +2649,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B4" s="4">
         <v>12</v>
@@ -3201,7 +2664,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G4" s="4">
         <v>-8</v>
@@ -3239,7 +2702,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B5" s="4">
         <v>12</v>
@@ -3254,7 +2717,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G5" s="4">
         <v>8</v>
@@ -3292,7 +2755,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="4" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B6" s="4">
         <v>16</v>
@@ -3307,7 +2770,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -3345,7 +2808,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="4" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B7" s="4">
         <v>16</v>
@@ -3360,7 +2823,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -3398,7 +2861,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B8" s="4">
         <v>16</v>
@@ -3413,7 +2876,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -3451,7 +2914,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B9" s="4">
         <v>16</v>
@@ -3466,7 +2929,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -3515,114 +2978,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="13.125" customWidth="1"/>
-    <col min="7" max="8" width="12.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1">
-      <c r="A1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="6" customFormat="1">
-      <c r="A2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="7" customFormat="1">
-      <c r="A3" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="4">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="4">
-        <v>100</v>
-      </c>
-      <c r="E3" s="4">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.75</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3644,16 +2999,16 @@
         <v>27</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1">
@@ -3661,21 +3016,21 @@
         <v>48</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="7" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B3" s="4">
         <v>0.4</v>
@@ -3701,7 +3056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -3720,47 +3075,47 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25">
       <c r="A1" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4">
         <v>0.4</v>
@@ -3780,7 +3135,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -3800,7 +3155,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B5" s="4">
         <v>0.3</v>
@@ -3820,7 +3175,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B6" s="4">
         <v>7.0000000000000007E-2</v>
@@ -3840,7 +3195,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B7" s="4">
         <v>0.1</v>
@@ -3860,7 +3215,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B8" s="4">
         <v>0.2</v>
@@ -3880,7 +3235,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B9" s="4">
         <v>0.15</v>
@@ -3900,7 +3255,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B10" s="4">
         <v>0.05</v>
@@ -3928,4 +3283,380 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14.25">
+      <c r="A1" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.25">
+      <c r="A2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>70</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>130</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>170</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>210</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>250</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>300</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>350</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>400</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>450</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>500</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>570</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>640</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>710</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>780</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>850</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>930</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>1010</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>1090</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>1170</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>1250</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>1350</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>1450</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>1550</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>1650</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>1800</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
move namebar to ui
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15615" tabRatio="735" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15615" tabRatio="735" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="176">
   <si>
     <t>地图宽</t>
   </si>
@@ -296,42 +296,12 @@
     <t>回血</t>
   </si>
   <si>
-    <t>名字显示字体</t>
-  </si>
-  <si>
-    <t>名字显示填充色</t>
-  </si>
-  <si>
-    <t>名字显示沟边色</t>
-  </si>
-  <si>
-    <t>名字显示沟边宽度</t>
-  </si>
-  <si>
-    <t>名字显示高度偏移</t>
-  </si>
-  <si>
     <t>武器</t>
   </si>
   <si>
     <t>hpRegen</t>
   </si>
   <si>
-    <t>namebar.font</t>
-  </si>
-  <si>
-    <t>namebar.fill</t>
-  </si>
-  <si>
-    <t>namebar.stroke</t>
-  </si>
-  <si>
-    <t>namebar.strokeThickness</t>
-  </si>
-  <si>
-    <t>namebar.yOffset</t>
-  </si>
-  <si>
     <t>weapons.0</t>
   </si>
   <si>
@@ -347,19 +317,7 @@
     <t>base</t>
   </si>
   <si>
-    <t>18px Arail</t>
-  </si>
-  <si>
-    <t>0x101010</t>
-  </si>
-  <si>
-    <t>0xf0f0f0</t>
-  </si>
-  <si>
     <t>twin</t>
-  </si>
-  <si>
-    <t>19px Arail</t>
   </si>
   <si>
     <t>twin-left</t>
@@ -692,7 +650,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,12 +678,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,7 +717,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -809,9 +761,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1254,36 +1203,36 @@
         <v>21</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="16" customFormat="1">
+    <row r="2" spans="1:6" s="15" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>26</v>
@@ -1385,7 +1334,7 @@
         <v>37</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>38</v>
@@ -1438,7 +1387,7 @@
         <v>53</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>54</v>
@@ -1447,13 +1396,13 @@
         <v>55</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="M2" s="13" t="s">
         <v>58</v>
@@ -1570,7 +1519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -1629,10 +1578,10 @@
         <v>37</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>38</v>
@@ -1697,10 +1646,10 @@
         <v>57</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="M2" s="13" t="s">
         <v>58</v>
@@ -1950,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -1978,16 +1927,12 @@
     <col min="20" max="20" width="11.625" customWidth="1"/>
     <col min="21" max="21" width="22.125" customWidth="1"/>
     <col min="22" max="22" width="21" customWidth="1"/>
-    <col min="23" max="23" width="12.625" customWidth="1"/>
-    <col min="24" max="25" width="14.5" customWidth="1"/>
-    <col min="26" max="26" width="22.625" customWidth="1"/>
-    <col min="27" max="27" width="16.375" customWidth="1"/>
-    <col min="28" max="28" width="11.125" customWidth="1"/>
-    <col min="29" max="29" width="11.625" customWidth="1"/>
-    <col min="30" max="31" width="11.125" customWidth="1"/>
+    <col min="23" max="23" width="11.125" customWidth="1"/>
+    <col min="24" max="24" width="11.625" customWidth="1"/>
+    <col min="25" max="26" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:26">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -2022,7 +1967,7 @@
         <v>88</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>38</v>
@@ -2054,35 +1999,20 @@
       <c r="V1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="X1" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y1" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z1" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA1" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE1" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" s="11" customFormat="1">
+      <c r="X1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="11" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>48</v>
       </c>
@@ -2114,10 +2044,10 @@
         <v>57</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="M2" s="13" t="s">
         <v>58</v>
@@ -2150,36 +2080,21 @@
         <v>67</v>
       </c>
       <c r="W2" s="13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="X2" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="Y2" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="Z2" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA2" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB2" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" s="7" customFormat="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="7" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4">
         <v>2.5</v>
@@ -2245,30 +2160,15 @@
         <v>10</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z3" s="4">
-        <v>2</v>
-      </c>
-      <c r="AA3" s="4">
-        <v>15</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-    </row>
-    <row r="4" spans="1:31">
+        <v>95</v>
+      </c>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B4" s="4">
         <v>2.5</v>
@@ -2334,30 +2234,15 @@
         <v>10</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z4" s="4">
-        <v>2</v>
-      </c>
-      <c r="AA4" s="4">
-        <v>18</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-    </row>
-    <row r="5" spans="1:31">
+        <v>98</v>
+      </c>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
@@ -2425,31 +2310,16 @@
         <v>10</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z5" s="4">
-        <v>2</v>
-      </c>
-      <c r="AA5" s="4">
-        <v>18</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE5" s="4" t="s">
-        <v>116</v>
+        <v>101</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2493,52 +2363,52 @@
         <v>27</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="11" customFormat="1">
@@ -2546,10 +2416,10 @@
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>50</v>
@@ -2561,42 +2431,42 @@
         <v>78</v>
       </c>
       <c r="G2" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>136</v>
-      </c>
       <c r="M2" s="13" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4">
         <v>15</v>
@@ -2611,7 +2481,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -2649,7 +2519,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B4" s="4">
         <v>12</v>
@@ -2664,7 +2534,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G4" s="4">
         <v>-8</v>
@@ -2702,7 +2572,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="4" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B5" s="4">
         <v>12</v>
@@ -2717,7 +2587,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G5" s="4">
         <v>8</v>
@@ -2755,7 +2625,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="4" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B6" s="4">
         <v>16</v>
@@ -2770,7 +2640,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -2808,7 +2678,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="4" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B7" s="4">
         <v>16</v>
@@ -2823,7 +2693,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -2861,7 +2731,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="4" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B8" s="4">
         <v>16</v>
@@ -2876,7 +2746,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -2914,7 +2784,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="4" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B9" s="4">
         <v>16</v>
@@ -2929,7 +2799,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -2999,16 +2869,16 @@
         <v>27</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1">
@@ -3016,21 +2886,21 @@
         <v>48</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="7" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4">
         <v>0.4</v>
@@ -3075,47 +2945,47 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25">
       <c r="A1" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B3" s="4">
         <v>0.4</v>
@@ -3135,7 +3005,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -3155,7 +3025,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B5" s="4">
         <v>0.3</v>
@@ -3175,7 +3045,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B6" s="4">
         <v>7.0000000000000007E-2</v>
@@ -3195,7 +3065,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B7" s="4">
         <v>0.1</v>
@@ -3215,7 +3085,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B8" s="4">
         <v>0.2</v>
@@ -3235,7 +3105,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B9" s="4">
         <v>0.15</v>
@@ -3255,7 +3125,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B10" s="4">
         <v>0.05</v>
@@ -3299,25 +3169,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25">
-      <c r="A1" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>183</v>
+      <c r="A1" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>

<commit_message>
world config move to package.json
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15615" tabRatio="735" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15615" tabRatio="735" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
-    <sheet name="configWorld" sheetId="2" r:id="rId2"/>
-    <sheet name="configBullets" sheetId="3" r:id="rId3"/>
-    <sheet name="configObstacles" sheetId="4" r:id="rId4"/>
-    <sheet name="configTanks" sheetId="5" r:id="rId5"/>
-    <sheet name="configWeapons" sheetId="6" r:id="rId6"/>
-    <sheet name="configDieAnimation" sheetId="8" r:id="rId7"/>
-    <sheet name="configPropAdd" sheetId="9" r:id="rId8"/>
-    <sheet name="configLevelUp" sheetId="10" r:id="rId9"/>
+    <sheet name="configBullets" sheetId="3" r:id="rId2"/>
+    <sheet name="configObstacles" sheetId="4" r:id="rId3"/>
+    <sheet name="configTanks" sheetId="5" r:id="rId4"/>
+    <sheet name="configWeapons" sheetId="6" r:id="rId5"/>
+    <sheet name="configDieAnimation" sheetId="8" r:id="rId6"/>
+    <sheet name="configPropAdd" sheetId="9" r:id="rId7"/>
+    <sheet name="configLevelUp" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="164">
   <si>
     <t>地图宽</t>
   </si>
@@ -90,24 +89,6 @@
   </si>
   <si>
     <t>0xcdcdcd</t>
-  </si>
-  <si>
-    <t>逻辑帧率</t>
-  </si>
-  <si>
-    <t>地图逻辑处理分格大小</t>
-  </si>
-  <si>
-    <t>中立物最大数量</t>
-  </si>
-  <si>
-    <t>frame</t>
-  </si>
-  <si>
-    <t>gridSize</t>
-  </si>
-  <si>
-    <t>maxObstaclesCount</t>
   </si>
   <si>
     <t>别名</t>
@@ -505,30 +486,6 @@
   </si>
   <si>
     <t>degree</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>碰撞检测保护时长(帧)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>unitCollideCheckFrame</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>syncRotationFrame</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>syncForceFrame</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>同步移动间隔(帧)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>同步旋转间隔(帧)</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -717,7 +674,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -761,9 +718,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1182,98 +1136,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.375" customWidth="1"/>
-    <col min="5" max="5" width="23.625" customWidth="1"/>
-    <col min="6" max="6" width="19.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1">
-      <c r="A1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="15" customFormat="1">
-      <c r="A2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="7" customFormat="1">
-      <c r="A3" s="4">
-        <v>30</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>128</v>
-      </c>
-      <c r="E3" s="4">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
@@ -1301,158 +1166,158 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="H1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="I1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="J1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="K1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="L1" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="N1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="O1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="Q1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="R1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1">
       <c r="A2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="J2" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="L2" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="K2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="R2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="M2" s="13" t="s">
+      <c r="S2" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="T2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="7" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4">
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G3" s="4">
         <v>25</v>
@@ -1515,7 +1380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V5"/>
   <sheetViews>
@@ -1548,143 +1413,143 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="J1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="Q1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="R1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1">
       <c r="A2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="J2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="M2" s="13" t="s">
+      <c r="S2" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="T2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="7" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
@@ -1693,13 +1558,13 @@
         <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E3" s="4">
         <v>2.5</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G3" s="4">
         <v>100</v>
@@ -1752,7 +1617,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
@@ -1761,13 +1626,13 @@
         <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E4" s="4">
         <v>2.5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G4" s="4">
         <v>400</v>
@@ -1820,7 +1685,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B5" s="4">
         <v>5</v>
@@ -1829,13 +1694,13 @@
         <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E5" s="4">
         <v>2.5</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G5" s="4">
         <v>1000</v>
@@ -1897,11 +1762,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="U1" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
@@ -1934,182 +1799,182 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="I1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="J1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="Q1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="R1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="W1" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="Z1" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="11" customFormat="1">
       <c r="A2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="K2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="M2" s="13" t="s">
+      <c r="S2" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="T2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>67</v>
-      </c>
       <c r="W2" s="13" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="X2" s="13" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Y2" s="13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z2" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="7" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B3" s="4">
         <v>2.5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4">
         <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G3" s="4">
         <v>1800</v>
@@ -2160,7 +2025,7 @@
         <v>10</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
@@ -2168,22 +2033,22 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B4" s="4">
         <v>2.5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4" s="4">
         <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G4" s="4">
         <v>2000</v>
@@ -2234,32 +2099,32 @@
         <v>10</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B5" s="4">
         <v>2.5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5" s="4">
         <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G5" s="4">
         <v>2200</v>
@@ -2310,16 +2175,16 @@
         <v>10</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2334,7 +2199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q9"/>
   <sheetViews>
@@ -2360,113 +2225,113 @@
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="J1" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="K1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="L1" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="11" customFormat="1">
       <c r="A2" s="13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="N2" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="I2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="K2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B3" s="4">
         <v>15</v>
@@ -2475,13 +2340,13 @@
         <v>35</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E3" s="4">
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -2490,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J3" s="4">
         <v>0</v>
@@ -2519,7 +2384,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B4" s="4">
         <v>12</v>
@@ -2528,13 +2393,13 @@
         <v>40</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G4" s="4">
         <v>-8</v>
@@ -2543,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J4" s="4">
         <v>0</v>
@@ -2572,7 +2437,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B5" s="4">
         <v>12</v>
@@ -2581,13 +2446,13 @@
         <v>40</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E5" s="4">
         <v>2</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G5" s="4">
         <v>8</v>
@@ -2596,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J5" s="4">
         <v>0</v>
@@ -2625,7 +2490,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B6" s="4">
         <v>16</v>
@@ -2634,13 +2499,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -2649,7 +2514,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J6" s="4">
         <v>0</v>
@@ -2678,7 +2543,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B7" s="4">
         <v>16</v>
@@ -2687,13 +2552,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E7" s="4">
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -2702,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J7" s="4">
         <v>90</v>
@@ -2731,7 +2596,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B8" s="4">
         <v>16</v>
@@ -2740,13 +2605,13 @@
         <v>38</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -2755,7 +2620,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J8" s="4">
         <v>180</v>
@@ -2784,7 +2649,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B9" s="4">
         <v>16</v>
@@ -2793,13 +2658,13 @@
         <v>38</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E9" s="4">
         <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -2808,7 +2673,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J9" s="4">
         <v>270</v>
@@ -2847,7 +2712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2866,41 +2731,41 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1">
       <c r="A2" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="7" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B3" s="4">
         <v>0.4</v>
@@ -2926,7 +2791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -2945,47 +2810,47 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B3" s="4">
         <v>0.4</v>
@@ -3005,7 +2870,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -3025,7 +2890,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B5" s="4">
         <v>0.3</v>
@@ -3045,7 +2910,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B6" s="4">
         <v>7.0000000000000007E-2</v>
@@ -3065,7 +2930,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B7" s="4">
         <v>0.1</v>
@@ -3085,7 +2950,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B8" s="4">
         <v>0.2</v>
@@ -3105,7 +2970,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B9" s="4">
         <v>0.15</v>
@@ -3125,7 +2990,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B10" s="4">
         <v>0.05</v>
@@ -3155,7 +3020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C32"/>
   <sheetViews>
@@ -3169,25 +3034,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25">
-      <c r="A1" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>169</v>
+      <c r="A1" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>

<commit_message>
1. obstacle & bullet use id as config key 2. weapon index in tank 3. tank sprite pivot
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15540" tabRatio="735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="configBullets" sheetId="3" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="configPropAdd" sheetId="9" r:id="rId5"/>
     <sheet name="configLevelUp" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="164">
-  <si>
-    <t>别名</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="161">
   <si>
     <t>勾边宽</t>
   </si>
@@ -83,9 +80,6 @@
     <t>自旋速度</t>
   </si>
   <si>
-    <t>alias</t>
-  </si>
-  <si>
     <t>view.edge.w</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>velocity.rv</t>
   </si>
   <si>
-    <t>normal</t>
-  </si>
-  <si>
     <t>0x555555</t>
   </si>
   <si>
@@ -170,19 +161,10 @@
     <t>view.color</t>
   </si>
   <si>
-    <t>triangle</t>
-  </si>
-  <si>
     <t>0xfc7676</t>
   </si>
   <si>
-    <t>quad</t>
-  </si>
-  <si>
     <t>0xffe869</t>
-  </si>
-  <si>
-    <t>pentagon</t>
   </si>
   <si>
     <t>0x768dfc</t>
@@ -569,31 +551,43 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>碰撞弹射速度</t>
+    <t>lifeSeconds</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>碰撞弹射抵抗速度</t>
+    <t>velocity.springBase</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>velocity.spring</t>
+    <t>velocity.springAdd</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>velocity.springResist</t>
+    <t>碰撞弹射基础速度</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>lifeSeconds</t>
+    <t>碰撞弹射加成速度</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -868,6 +862,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="15">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -875,14 +870,13 @@
     <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1173,189 +1167,189 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" customWidth="1"/>
+    <col min="8" max="8" width="7.125" customWidth="1"/>
     <col min="9" max="9" width="7.5" customWidth="1"/>
     <col min="10" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" customWidth="1"/>
-    <col min="14" max="15" width="16.1640625" customWidth="1"/>
-    <col min="16" max="17" width="17.1640625" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" customWidth="1"/>
-    <col min="19" max="19" width="17.1640625" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" customWidth="1"/>
-    <col min="21" max="21" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.125" customWidth="1"/>
+    <col min="14" max="15" width="16.125" customWidth="1"/>
+    <col min="16" max="17" width="17.125" customWidth="1"/>
+    <col min="18" max="18" width="16.125" customWidth="1"/>
+    <col min="19" max="19" width="17.125" customWidth="1"/>
+    <col min="20" max="20" width="11.625" customWidth="1"/>
+    <col min="21" max="21" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="U1" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="9" customFormat="1">
       <c r="A2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="G2" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>36</v>
-      </c>
       <c r="U2" s="11" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="6" customFormat="1">
-      <c r="A3" s="4" t="s">
-        <v>37</v>
+      <c r="A3" s="4">
+        <v>2010</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4">
         <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="4">
         <v>2.5</v>
@@ -1400,10 +1394,10 @@
         <v>0</v>
       </c>
       <c r="U3" s="4">
-        <v>875</v>
+        <v>30</v>
       </c>
       <c r="V3" s="4">
-        <v>875</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1419,175 +1413,175 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
+    <col min="7" max="7" width="7.125" customWidth="1"/>
     <col min="8" max="8" width="7.5" customWidth="1"/>
     <col min="9" max="10" width="8.5" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" customWidth="1"/>
-    <col min="14" max="15" width="16.1640625" customWidth="1"/>
-    <col min="16" max="17" width="17.1640625" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" customWidth="1"/>
-    <col min="19" max="19" width="16.33203125" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" customWidth="1"/>
-    <col min="21" max="21" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.125" customWidth="1"/>
+    <col min="14" max="15" width="16.125" customWidth="1"/>
+    <col min="16" max="17" width="17.125" customWidth="1"/>
+    <col min="18" max="18" width="16.125" customWidth="1"/>
+    <col min="19" max="19" width="16.375" customWidth="1"/>
+    <col min="20" max="20" width="11.625" customWidth="1"/>
+    <col min="21" max="21" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="U1" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="9" customFormat="1">
       <c r="A2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="G2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>36</v>
-      </c>
       <c r="U2" s="11" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="6" customFormat="1">
-      <c r="A3" s="4" t="s">
-        <v>48</v>
+      <c r="A3" s="4">
+        <v>301</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
@@ -1596,13 +1590,13 @@
         <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="4">
         <v>2.5</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G3" s="4">
         <v>100</v>
@@ -1647,15 +1641,15 @@
         <v>0.5</v>
       </c>
       <c r="U3" s="4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="V3" s="4">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:22">
-      <c r="A4" s="4" t="s">
-        <v>50</v>
+      <c r="A4" s="4">
+        <v>302</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
@@ -1664,13 +1658,13 @@
         <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4" s="4">
         <v>2.5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G4" s="4">
         <v>400</v>
@@ -1715,15 +1709,15 @@
         <v>0.5</v>
       </c>
       <c r="U4" s="4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="V4" s="4">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="4" t="s">
-        <v>52</v>
+      <c r="A5" s="4">
+        <v>303</v>
       </c>
       <c r="B5" s="4">
         <v>5</v>
@@ -1732,13 +1726,13 @@
         <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E5" s="4">
         <v>2.5</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G5" s="4">
         <v>1000</v>
@@ -1783,10 +1777,10 @@
         <v>0.5</v>
       </c>
       <c r="U5" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="V5" s="4">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1801,226 +1795,226 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF22" sqref="AF22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="10.375" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="8.5" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="21" width="11.1640625" customWidth="1"/>
-    <col min="22" max="22" width="17.1640625" customWidth="1"/>
-    <col min="23" max="24" width="16.1640625" customWidth="1"/>
-    <col min="25" max="26" width="17.1640625" customWidth="1"/>
-    <col min="27" max="27" width="16.1640625" customWidth="1"/>
-    <col min="28" max="28" width="17.1640625" customWidth="1"/>
-    <col min="29" max="29" width="11.6640625" customWidth="1"/>
-    <col min="30" max="30" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.625" customWidth="1"/>
+    <col min="10" max="13" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.125" customWidth="1"/>
+    <col min="15" max="15" width="11.625" customWidth="1"/>
+    <col min="16" max="21" width="11.125" customWidth="1"/>
+    <col min="22" max="22" width="17.125" customWidth="1"/>
+    <col min="23" max="24" width="16.125" customWidth="1"/>
+    <col min="25" max="26" width="17.125" customWidth="1"/>
+    <col min="27" max="27" width="16.125" customWidth="1"/>
+    <col min="28" max="28" width="17.125" customWidth="1"/>
+    <col min="29" max="29" width="11.625" customWidth="1"/>
+    <col min="30" max="30" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="X1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AB1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AC1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="AD1" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AE1" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:31" s="9" customFormat="1">
       <c r="A2" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="F2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="V2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="W2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="R2" s="11" t="s">
+      <c r="X2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE2" s="11" t="s">
         <v>155</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE2" s="11" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:31" s="6" customFormat="1">
@@ -2046,7 +2040,7 @@
         <v>99999</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I3" s="4">
         <v>5</v>
@@ -2099,10 +2093,10 @@
         <v>0</v>
       </c>
       <c r="AD3" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE3" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:31">
@@ -2128,7 +2122,7 @@
         <v>99999</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I4" s="4">
         <v>15</v>
@@ -2179,10 +2173,10 @@
         <v>0</v>
       </c>
       <c r="AD4" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE4" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -2208,7 +2202,7 @@
         <v>99999</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="I5" s="4">
         <v>15</v>
@@ -2259,10 +2253,10 @@
         <v>0</v>
       </c>
       <c r="AD5" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE5" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -2288,7 +2282,7 @@
         <v>99999</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I6" s="4">
         <v>15</v>
@@ -2339,10 +2333,10 @@
         <v>0</v>
       </c>
       <c r="AD6" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE6" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -2368,7 +2362,7 @@
         <v>99999</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="I7" s="4">
         <v>15</v>
@@ -2415,10 +2409,10 @@
         <v>0</v>
       </c>
       <c r="AD7" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE7" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -2444,7 +2438,7 @@
         <v>99999</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="I8" s="4">
         <v>30</v>
@@ -2491,10 +2485,10 @@
         <v>0</v>
       </c>
       <c r="AD8" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE8" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -2520,7 +2514,7 @@
         <v>99999</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I9" s="4">
         <v>30</v>
@@ -2569,10 +2563,10 @@
         <v>0</v>
       </c>
       <c r="AD9" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE9" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -2598,7 +2592,7 @@
         <v>99999</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I10" s="4">
         <v>30</v>
@@ -2651,10 +2645,10 @@
         <v>0</v>
       </c>
       <c r="AD10" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE10" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -2680,7 +2674,7 @@
         <v>99999</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I11" s="4">
         <v>30</v>
@@ -2733,10 +2727,10 @@
         <v>0</v>
       </c>
       <c r="AD11" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE11" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -2762,7 +2756,7 @@
         <v>99999</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I12" s="4">
         <v>30</v>
@@ -2815,10 +2809,10 @@
         <v>0</v>
       </c>
       <c r="AD12" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE12" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -2844,7 +2838,7 @@
         <v>99999</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I13" s="4">
         <v>30</v>
@@ -2897,10 +2891,10 @@
         <v>0</v>
       </c>
       <c r="AD13" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE13" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -2926,7 +2920,7 @@
         <v>99999</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I14" s="4">
         <v>30</v>
@@ -2973,10 +2967,10 @@
         <v>0</v>
       </c>
       <c r="AD14" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE14" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -3002,7 +2996,7 @@
         <v>99999</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I15" s="4">
         <v>30</v>
@@ -3049,10 +3043,10 @@
         <v>0</v>
       </c>
       <c r="AD15" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE15" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:31">
@@ -3078,7 +3072,7 @@
         <v>99999</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -3121,10 +3115,10 @@
         <v>0</v>
       </c>
       <c r="AD16" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE16" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:31">
@@ -3150,7 +3144,7 @@
         <v>99999</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -3195,10 +3189,10 @@
         <v>0</v>
       </c>
       <c r="AD17" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE17" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:31">
@@ -3224,7 +3218,7 @@
         <v>99999</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -3275,10 +3269,10 @@
         <v>0</v>
       </c>
       <c r="AD18" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE18" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:31">
@@ -3304,7 +3298,7 @@
         <v>99999</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -3361,10 +3355,10 @@
         <v>0</v>
       </c>
       <c r="AD19" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE19" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:31">
@@ -3390,7 +3384,7 @@
         <v>99999</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -3437,10 +3431,10 @@
         <v>0</v>
       </c>
       <c r="AD20" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE20" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:31">
@@ -3466,7 +3460,7 @@
         <v>99999</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -3517,10 +3511,10 @@
         <v>0</v>
       </c>
       <c r="AD21" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE21" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:31">
@@ -3546,7 +3540,7 @@
         <v>99999</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -3589,10 +3583,10 @@
         <v>0</v>
       </c>
       <c r="AD22" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE22" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:31">
@@ -3618,7 +3612,7 @@
         <v>99999</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -3659,10 +3653,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE23" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:31">
@@ -3688,7 +3682,7 @@
         <v>99999</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -3729,10 +3723,10 @@
         <v>0</v>
       </c>
       <c r="AD24" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE24" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:31">
@@ -3758,7 +3752,7 @@
         <v>99999</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -3811,10 +3805,10 @@
         <v>0</v>
       </c>
       <c r="AD25" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE25" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:31">
@@ -3840,7 +3834,7 @@
         <v>99999</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I26" s="4">
         <v>30</v>
@@ -3891,10 +3885,10 @@
         <v>0</v>
       </c>
       <c r="AD26" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE26" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:31">
@@ -3920,7 +3914,7 @@
         <v>99999</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -3967,10 +3961,10 @@
         <v>0</v>
       </c>
       <c r="AD27" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE27" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:31">
@@ -3996,7 +3990,7 @@
         <v>99999</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -4043,10 +4037,10 @@
         <v>0</v>
       </c>
       <c r="AD28" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE28" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:31">
@@ -4072,7 +4066,7 @@
         <v>99999</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -4115,10 +4109,10 @@
         <v>0</v>
       </c>
       <c r="AD29" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE29" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:31">
@@ -4144,7 +4138,7 @@
         <v>99999</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -4193,10 +4187,10 @@
         <v>0</v>
       </c>
       <c r="AD30" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE30" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:31">
@@ -4222,7 +4216,7 @@
         <v>99999</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -4271,10 +4265,10 @@
         <v>0</v>
       </c>
       <c r="AD31" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE31" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:31">
@@ -4300,7 +4294,7 @@
         <v>99999</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -4351,10 +4345,10 @@
         <v>0</v>
       </c>
       <c r="AD32" s="4">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="AE32" s="4">
-        <v>750</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4370,112 +4364,112 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N200"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:F79"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="20"/>
-    <col min="5" max="5" width="11.6640625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="8" width="9.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="20"/>
+    <col min="5" max="5" width="11.625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="8" width="9.875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.875" customWidth="1"/>
+    <col min="10" max="10" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.875" customWidth="1"/>
+    <col min="12" max="12" width="15.125" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1">
       <c r="A1" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1">
       <c r="A2" s="11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
       <c r="I2" s="15" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4">
         <v>1010</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
+      <c r="B3" s="4">
+        <v>2010</v>
       </c>
       <c r="C3" s="19">
         <v>2010</v>
@@ -4521,8 +4515,8 @@
       <c r="A4" s="4">
         <v>1020</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
+      <c r="B4" s="4">
+        <v>2010</v>
       </c>
       <c r="C4" s="19">
         <v>2020</v>
@@ -4566,8 +4560,8 @@
       <c r="A5" s="4">
         <v>1030</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>37</v>
+      <c r="B5" s="4">
+        <v>2010</v>
       </c>
       <c r="C5" s="19">
         <v>2030</v>
@@ -4611,8 +4605,8 @@
       <c r="A6" s="4">
         <v>1031</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>37</v>
+      <c r="B6" s="4">
+        <v>2010</v>
       </c>
       <c r="C6" s="19">
         <v>2030</v>
@@ -4656,8 +4650,8 @@
       <c r="A7" s="4">
         <v>1040</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
+      <c r="B7" s="4">
+        <v>2010</v>
       </c>
       <c r="C7" s="19">
         <v>2040</v>
@@ -4701,8 +4695,8 @@
       <c r="A8" s="4">
         <v>1041</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
+      <c r="B8" s="4">
+        <v>2010</v>
       </c>
       <c r="C8" s="19">
         <v>2040</v>
@@ -4746,8 +4740,8 @@
       <c r="A9" s="4">
         <v>1050</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>37</v>
+      <c r="B9" s="4">
+        <v>2010</v>
       </c>
       <c r="C9" s="19">
         <v>2050</v>
@@ -4791,8 +4785,8 @@
       <c r="A10" s="4">
         <v>1060</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>37</v>
+      <c r="B10" s="4">
+        <v>2010</v>
       </c>
       <c r="C10" s="19">
         <v>2060</v>
@@ -4836,8 +4830,8 @@
       <c r="A11" s="4">
         <v>1070</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>37</v>
+      <c r="B11" s="4">
+        <v>2010</v>
       </c>
       <c r="C11" s="19">
         <v>2070</v>
@@ -4881,8 +4875,8 @@
       <c r="A12" s="4">
         <v>1071</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>37</v>
+      <c r="B12" s="4">
+        <v>2010</v>
       </c>
       <c r="C12" s="19">
         <v>2071</v>
@@ -4926,8 +4920,8 @@
       <c r="A13" s="4">
         <v>1080</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>37</v>
+      <c r="B13" s="4">
+        <v>2010</v>
       </c>
       <c r="C13" s="19">
         <v>2081</v>
@@ -4971,8 +4965,8 @@
       <c r="A14" s="4">
         <v>1081</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
+      <c r="B14" s="4">
+        <v>2010</v>
       </c>
       <c r="C14" s="19">
         <v>2080</v>
@@ -5016,8 +5010,8 @@
       <c r="A15" s="4">
         <v>1082</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>37</v>
+      <c r="B15" s="4">
+        <v>2010</v>
       </c>
       <c r="C15" s="19">
         <v>2080</v>
@@ -5061,8 +5055,8 @@
       <c r="A16" s="4">
         <v>1090</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>37</v>
+      <c r="B16" s="4">
+        <v>2010</v>
       </c>
       <c r="C16" s="19">
         <v>2090</v>
@@ -5106,8 +5100,8 @@
       <c r="A17" s="4">
         <v>1091</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>37</v>
+      <c r="B17" s="4">
+        <v>2010</v>
       </c>
       <c r="C17" s="19">
         <v>2090</v>
@@ -5151,8 +5145,8 @@
       <c r="A18" s="4">
         <v>1092</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>37</v>
+      <c r="B18" s="4">
+        <v>2010</v>
       </c>
       <c r="C18" s="19">
         <v>2090</v>
@@ -5196,8 +5190,8 @@
       <c r="A19" s="4">
         <v>1093</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>37</v>
+      <c r="B19" s="4">
+        <v>2010</v>
       </c>
       <c r="C19" s="19">
         <v>2090</v>
@@ -5241,8 +5235,8 @@
       <c r="A20" s="4">
         <v>1100</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>37</v>
+      <c r="B20" s="4">
+        <v>2010</v>
       </c>
       <c r="C20" s="19">
         <v>2100</v>
@@ -5286,8 +5280,8 @@
       <c r="A21" s="4">
         <v>1101</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>37</v>
+      <c r="B21" s="4">
+        <v>2010</v>
       </c>
       <c r="C21" s="19">
         <v>2100</v>
@@ -5331,8 +5325,8 @@
       <c r="A22" s="4">
         <v>1102</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>37</v>
+      <c r="B22" s="4">
+        <v>2010</v>
       </c>
       <c r="C22" s="19">
         <v>2100</v>
@@ -5376,8 +5370,8 @@
       <c r="A23" s="4">
         <v>1103</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>37</v>
+      <c r="B23" s="4">
+        <v>2010</v>
       </c>
       <c r="C23" s="19">
         <v>2100</v>
@@ -5421,8 +5415,8 @@
       <c r="A24" s="4">
         <v>1110</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>37</v>
+      <c r="B24" s="4">
+        <v>2010</v>
       </c>
       <c r="C24" s="19">
         <v>2110</v>
@@ -5466,8 +5460,8 @@
       <c r="A25" s="4">
         <v>1111</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>37</v>
+      <c r="B25" s="4">
+        <v>2010</v>
       </c>
       <c r="C25" s="19">
         <v>2110</v>
@@ -5511,8 +5505,8 @@
       <c r="A26" s="4">
         <v>1112</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>37</v>
+      <c r="B26" s="4">
+        <v>2010</v>
       </c>
       <c r="C26" s="19">
         <v>2110</v>
@@ -5556,8 +5550,8 @@
       <c r="A27" s="4">
         <v>1120</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>37</v>
+      <c r="B27" s="4">
+        <v>2010</v>
       </c>
       <c r="C27" s="19">
         <v>2120</v>
@@ -5601,8 +5595,8 @@
       <c r="A28" s="4">
         <v>1140</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>37</v>
+      <c r="B28" s="4">
+        <v>2010</v>
       </c>
       <c r="C28" s="19">
         <v>2140</v>
@@ -5646,8 +5640,8 @@
       <c r="A29" s="4">
         <v>1150</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>37</v>
+      <c r="B29" s="4">
+        <v>2010</v>
       </c>
       <c r="C29" s="19">
         <v>2150</v>
@@ -5691,8 +5685,8 @@
       <c r="A30" s="4">
         <v>1151</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>37</v>
+      <c r="B30" s="4">
+        <v>2010</v>
       </c>
       <c r="C30" s="19">
         <v>2151</v>
@@ -5736,8 +5730,8 @@
       <c r="A31" s="4">
         <v>1160</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>37</v>
+      <c r="B31" s="4">
+        <v>2010</v>
       </c>
       <c r="C31" s="19">
         <v>2161</v>
@@ -5781,8 +5775,8 @@
       <c r="A32" s="4">
         <v>1161</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>37</v>
+      <c r="B32" s="4">
+        <v>2010</v>
       </c>
       <c r="C32" s="19">
         <v>2160</v>
@@ -5826,8 +5820,8 @@
       <c r="A33" s="4">
         <v>1162</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>37</v>
+      <c r="B33" s="4">
+        <v>2010</v>
       </c>
       <c r="C33" s="19">
         <v>2160</v>
@@ -5871,8 +5865,8 @@
       <c r="A34" s="4">
         <v>1163</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>37</v>
+      <c r="B34" s="4">
+        <v>2010</v>
       </c>
       <c r="C34" s="19">
         <v>2160</v>
@@ -5916,8 +5910,8 @@
       <c r="A35" s="4">
         <v>1164</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>37</v>
+      <c r="B35" s="4">
+        <v>2010</v>
       </c>
       <c r="C35" s="19">
         <v>2160</v>
@@ -5961,8 +5955,8 @@
       <c r="A36" s="4">
         <v>1170</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>37</v>
+      <c r="B36" s="4">
+        <v>2010</v>
       </c>
       <c r="C36" s="19">
         <v>2170</v>
@@ -6006,8 +6000,8 @@
       <c r="A37" s="4">
         <v>1171</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>37</v>
+      <c r="B37" s="4">
+        <v>2010</v>
       </c>
       <c r="C37" s="19">
         <v>2170</v>
@@ -6051,8 +6045,8 @@
       <c r="A38" s="4">
         <v>1172</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>37</v>
+      <c r="B38" s="4">
+        <v>2010</v>
       </c>
       <c r="C38" s="19">
         <v>2170</v>
@@ -6096,8 +6090,8 @@
       <c r="A39" s="4">
         <v>1173</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>37</v>
+      <c r="B39" s="4">
+        <v>2010</v>
       </c>
       <c r="C39" s="19">
         <v>2170</v>
@@ -6141,8 +6135,8 @@
       <c r="A40" s="4">
         <v>1174</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>37</v>
+      <c r="B40" s="4">
+        <v>2010</v>
       </c>
       <c r="C40" s="19">
         <v>2170</v>
@@ -6186,8 +6180,8 @@
       <c r="A41" s="4">
         <v>1175</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>37</v>
+      <c r="B41" s="4">
+        <v>2010</v>
       </c>
       <c r="C41" s="19">
         <v>2170</v>
@@ -6231,8 +6225,8 @@
       <c r="A42" s="4">
         <v>1176</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>37</v>
+      <c r="B42" s="4">
+        <v>2010</v>
       </c>
       <c r="C42" s="19">
         <v>2170</v>
@@ -6276,8 +6270,8 @@
       <c r="A43" s="4">
         <v>1177</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>37</v>
+      <c r="B43" s="4">
+        <v>2010</v>
       </c>
       <c r="C43" s="19">
         <v>2170</v>
@@ -6321,8 +6315,8 @@
       <c r="A44" s="4">
         <v>1180</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>37</v>
+      <c r="B44" s="4">
+        <v>2010</v>
       </c>
       <c r="C44" s="19">
         <v>2180</v>
@@ -6366,8 +6360,8 @@
       <c r="A45" s="4">
         <v>1181</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>37</v>
+      <c r="B45" s="4">
+        <v>2010</v>
       </c>
       <c r="C45" s="19">
         <v>2180</v>
@@ -6411,8 +6405,8 @@
       <c r="A46" s="4">
         <v>1182</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>37</v>
+      <c r="B46" s="4">
+        <v>2010</v>
       </c>
       <c r="C46" s="19">
         <v>2180</v>
@@ -6456,8 +6450,8 @@
       <c r="A47" s="4">
         <v>1190</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>37</v>
+      <c r="B47" s="4">
+        <v>2010</v>
       </c>
       <c r="C47" s="19">
         <v>2190</v>
@@ -6501,8 +6495,8 @@
       <c r="A48" s="4">
         <v>1191</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>37</v>
+      <c r="B48" s="4">
+        <v>2010</v>
       </c>
       <c r="C48" s="19">
         <v>2190</v>
@@ -6546,8 +6540,8 @@
       <c r="A49" s="4">
         <v>1192</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>37</v>
+      <c r="B49" s="4">
+        <v>2010</v>
       </c>
       <c r="C49" s="19">
         <v>2190</v>
@@ -6591,8 +6585,8 @@
       <c r="A50" s="4">
         <v>1193</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>37</v>
+      <c r="B50" s="4">
+        <v>2010</v>
       </c>
       <c r="C50" s="19">
         <v>2190</v>
@@ -6636,8 +6630,8 @@
       <c r="A51" s="4">
         <v>1194</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>37</v>
+      <c r="B51" s="4">
+        <v>2010</v>
       </c>
       <c r="C51" s="19">
         <v>2190</v>
@@ -6681,8 +6675,8 @@
       <c r="A52" s="4">
         <v>1200</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>37</v>
+      <c r="B52" s="4">
+        <v>2010</v>
       </c>
       <c r="C52" s="19">
         <v>2200</v>
@@ -6726,8 +6720,8 @@
       <c r="A53" s="4">
         <v>1230</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>37</v>
+      <c r="B53" s="4">
+        <v>2010</v>
       </c>
       <c r="C53" s="19">
         <v>2230</v>
@@ -6771,8 +6765,8 @@
       <c r="A54" s="4">
         <v>1231</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>37</v>
+      <c r="B54" s="4">
+        <v>2010</v>
       </c>
       <c r="C54" s="19">
         <v>2230</v>
@@ -6816,8 +6810,8 @@
       <c r="A55" s="4">
         <v>1232</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>37</v>
+      <c r="B55" s="4">
+        <v>2010</v>
       </c>
       <c r="C55" s="19">
         <v>2230</v>
@@ -6861,8 +6855,8 @@
       <c r="A56" s="4">
         <v>1233</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>37</v>
+      <c r="B56" s="4">
+        <v>2010</v>
       </c>
       <c r="C56" s="19">
         <v>2230</v>
@@ -6906,8 +6900,8 @@
       <c r="A57" s="4">
         <v>1234</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>37</v>
+      <c r="B57" s="4">
+        <v>2010</v>
       </c>
       <c r="C57" s="19">
         <v>2230</v>
@@ -6951,8 +6945,8 @@
       <c r="A58" s="4">
         <v>1235</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>37</v>
+      <c r="B58" s="4">
+        <v>2010</v>
       </c>
       <c r="C58" s="19">
         <v>2230</v>
@@ -6996,8 +6990,8 @@
       <c r="A59" s="4">
         <v>1240</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>37</v>
+      <c r="B59" s="4">
+        <v>2010</v>
       </c>
       <c r="C59" s="19">
         <v>2240</v>
@@ -7041,8 +7035,8 @@
       <c r="A60" s="4">
         <v>1250</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>37</v>
+      <c r="B60" s="4">
+        <v>2010</v>
       </c>
       <c r="C60" s="19">
         <v>2250</v>
@@ -7086,8 +7080,8 @@
       <c r="A61" s="4">
         <v>1251</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>37</v>
+      <c r="B61" s="4">
+        <v>2010</v>
       </c>
       <c r="C61" s="19">
         <v>2250</v>
@@ -7131,8 +7125,8 @@
       <c r="A62" s="4">
         <v>1252</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>37</v>
+      <c r="B62" s="4">
+        <v>2010</v>
       </c>
       <c r="C62" s="19">
         <v>2250</v>
@@ -7176,8 +7170,8 @@
       <c r="A63" s="4">
         <v>1260</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>37</v>
+      <c r="B63" s="4">
+        <v>2010</v>
       </c>
       <c r="C63" s="19">
         <v>2260</v>
@@ -7221,8 +7215,8 @@
       <c r="A64" s="4">
         <v>1261</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>37</v>
+      <c r="B64" s="4">
+        <v>2010</v>
       </c>
       <c r="C64" s="19">
         <v>2261</v>
@@ -7266,8 +7260,8 @@
       <c r="A65" s="4">
         <v>1262</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>37</v>
+      <c r="B65" s="4">
+        <v>2010</v>
       </c>
       <c r="C65" s="19">
         <v>2261</v>
@@ -7311,8 +7305,8 @@
       <c r="A66" s="4">
         <v>1270</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>37</v>
+      <c r="B66" s="4">
+        <v>2010</v>
       </c>
       <c r="C66" s="19">
         <v>2270</v>
@@ -7356,8 +7350,8 @@
       <c r="A67" s="4">
         <v>1280</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>37</v>
+      <c r="B67" s="4">
+        <v>2010</v>
       </c>
       <c r="C67" s="19">
         <v>2280</v>
@@ -7401,8 +7395,8 @@
       <c r="A68" s="4">
         <v>1281</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>37</v>
+      <c r="B68" s="4">
+        <v>2010</v>
       </c>
       <c r="C68" s="19">
         <v>2280</v>
@@ -7446,8 +7440,8 @@
       <c r="A69" s="4">
         <v>1282</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>37</v>
+      <c r="B69" s="4">
+        <v>2010</v>
       </c>
       <c r="C69" s="19">
         <v>2280</v>
@@ -7491,8 +7485,8 @@
       <c r="A70" s="4">
         <v>1283</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>37</v>
+      <c r="B70" s="4">
+        <v>2010</v>
       </c>
       <c r="C70" s="19">
         <v>2280</v>
@@ -7536,8 +7530,8 @@
       <c r="A71" s="4">
         <v>1290</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>37</v>
+      <c r="B71" s="4">
+        <v>2010</v>
       </c>
       <c r="C71" s="19">
         <v>2290</v>
@@ -7581,8 +7575,8 @@
       <c r="A72" s="4">
         <v>1291</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>37</v>
+      <c r="B72" s="4">
+        <v>2010</v>
       </c>
       <c r="C72" s="19">
         <v>2290</v>
@@ -7626,8 +7620,8 @@
       <c r="A73" s="4">
         <v>1292</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>37</v>
+      <c r="B73" s="4">
+        <v>2010</v>
       </c>
       <c r="C73" s="19">
         <v>2290</v>
@@ -7671,8 +7665,8 @@
       <c r="A74" s="4">
         <v>1293</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>37</v>
+      <c r="B74" s="4">
+        <v>2010</v>
       </c>
       <c r="C74" s="19">
         <v>2290</v>
@@ -7716,8 +7710,8 @@
       <c r="A75" s="4">
         <v>1300</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>37</v>
+      <c r="B75" s="4">
+        <v>2010</v>
       </c>
       <c r="C75" s="19">
         <v>2301</v>
@@ -7761,8 +7755,8 @@
       <c r="A76" s="4">
         <v>1301</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>37</v>
+      <c r="B76" s="4">
+        <v>2010</v>
       </c>
       <c r="C76" s="19">
         <v>2300</v>
@@ -7806,8 +7800,8 @@
       <c r="A77" s="4">
         <v>1302</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>37</v>
+      <c r="B77" s="4">
+        <v>2010</v>
       </c>
       <c r="C77" s="19">
         <v>2300</v>
@@ -7851,8 +7845,8 @@
       <c r="A78" s="4">
         <v>1303</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>37</v>
+      <c r="B78" s="4">
+        <v>2010</v>
       </c>
       <c r="C78" s="19">
         <v>2300</v>
@@ -7896,8 +7890,8 @@
       <c r="A79" s="4">
         <v>1304</v>
       </c>
-      <c r="B79" s="4" t="s">
-        <v>37</v>
+      <c r="B79" s="4">
+        <v>2010</v>
       </c>
       <c r="C79" s="19">
         <v>2300</v>
@@ -9886,65 +9880,65 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="3" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.875" customWidth="1"/>
+    <col min="2" max="3" width="10.125" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.125" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6" ht="14.25">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.25">
+      <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B3" s="4">
         <v>0.4</v>
@@ -9964,7 +9958,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -9984,7 +9978,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B5" s="4">
         <v>0.3</v>
@@ -10004,7 +9998,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B6" s="4">
         <v>7.0000000000000007E-2</v>
@@ -10024,7 +10018,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B7" s="4">
         <v>0.1</v>
@@ -10044,7 +10038,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B8" s="4">
         <v>0.2</v>
@@ -10064,7 +10058,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B9" s="4">
         <v>0.15</v>
@@ -10084,7 +10078,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B10" s="4">
         <v>0.05</v>
@@ -10115,38 +10109,38 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5"/>
   <cols>
     <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="14.25">
       <c r="A1" s="13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -10200,9 +10194,6 @@
       <c r="B7">
         <v>70</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
@@ -10310,9 +10301,6 @@
       <c r="B17">
         <v>500</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
@@ -10474,9 +10462,6 @@
       </c>
       <c r="B32">
         <v>1800</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>